<commit_message>
Formatted colors in error analysis. Checked the results.
</commit_message>
<xml_diff>
--- a/Dataset/Error analysis/GC_Test_with_predictions.xlsx
+++ b/Dataset/Error analysis/GC_Test_with_predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slivk\OneDrive\CleanCaDET\Deliverables\C# AI detector performance report\code\ML-code-smell-CSharp\Dataset\Error analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD378BC4-7E0B-4846-9EBB-E9DE05C928C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D12678-0BBF-4BCD-A1FA-E6A6FFEE340E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24160" yWindow="-2480" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prediction results" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="402">
   <si>
     <t>Code Snippet ID</t>
   </si>
@@ -1245,7 +1245,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1274,8 +1274,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1284,19 +1290,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1348,18 +1348,30 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1740,9 +1752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1771,10 +1783,10 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>384</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -2736,12 +2748,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
@@ -2781,12 +2793,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
@@ -2826,12 +2838,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
@@ -2871,12 +2883,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
@@ -2916,12 +2928,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
@@ -2961,12 +2973,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
@@ -3006,12 +3018,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
@@ -3051,12 +3063,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
@@ -3096,12 +3108,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
@@ -3141,12 +3153,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
@@ -3186,12 +3198,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
@@ -3231,12 +3243,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
@@ -3276,12 +3288,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
@@ -3321,12 +3333,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
@@ -3366,12 +3378,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
@@ -3411,12 +3423,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
@@ -3456,12 +3468,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
@@ -3501,12 +3513,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
@@ -3546,12 +3558,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
@@ -3591,12 +3603,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
@@ -3636,12 +3648,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
@@ -3681,12 +3693,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
@@ -3726,12 +3738,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
@@ -3771,12 +3783,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
@@ -3816,12 +3828,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
@@ -3861,12 +3873,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
@@ -3906,12 +3918,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
-      <c r="P50" s="6"/>
-      <c r="Q50" s="6"/>
-      <c r="R50" s="6"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
@@ -3951,12 +3963,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
@@ -3996,12 +4008,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
@@ -4041,12 +4053,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
@@ -4086,12 +4098,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
@@ -4131,12 +4143,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
@@ -4176,12 +4188,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="6"/>
-      <c r="Q56" s="6"/>
-      <c r="R56" s="6"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
@@ -4221,12 +4233,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
-      <c r="P57" s="6"/>
-      <c r="Q57" s="6"/>
-      <c r="R57" s="6"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
@@ -4266,12 +4278,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M58" s="6"/>
-      <c r="N58" s="6"/>
-      <c r="O58" s="6"/>
-      <c r="P58" s="6"/>
-      <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
@@ -4311,12 +4323,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M59" s="6"/>
-      <c r="N59" s="6"/>
-      <c r="O59" s="6"/>
-      <c r="P59" s="6"/>
-      <c r="Q59" s="6"/>
-      <c r="R59" s="6"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
@@ -4356,12 +4368,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M60" s="6"/>
-      <c r="N60" s="6"/>
-      <c r="O60" s="6"/>
-      <c r="P60" s="6"/>
-      <c r="Q60" s="6"/>
-      <c r="R60" s="6"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
@@ -4401,12 +4413,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
-      <c r="P61" s="6"/>
-      <c r="Q61" s="6"/>
-      <c r="R61" s="6"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
@@ -4446,12 +4458,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M62" s="6"/>
-      <c r="N62" s="6"/>
-      <c r="O62" s="6"/>
-      <c r="P62" s="6"/>
-      <c r="Q62" s="6"/>
-      <c r="R62" s="6"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
@@ -4491,12 +4503,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M63" s="6"/>
-      <c r="N63" s="6"/>
-      <c r="O63" s="6"/>
-      <c r="P63" s="6"/>
-      <c r="Q63" s="6"/>
-      <c r="R63" s="6"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
@@ -4536,12 +4548,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M64" s="6"/>
-      <c r="N64" s="6"/>
-      <c r="O64" s="6"/>
-      <c r="P64" s="6"/>
-      <c r="Q64" s="6"/>
-      <c r="R64" s="6"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
@@ -4581,12 +4593,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M65" s="6"/>
-      <c r="N65" s="6"/>
-      <c r="O65" s="6"/>
-      <c r="P65" s="6"/>
-      <c r="Q65" s="6"/>
-      <c r="R65" s="6"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
@@ -4626,12 +4638,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M66" s="6"/>
-      <c r="N66" s="6"/>
-      <c r="O66" s="6"/>
-      <c r="P66" s="6"/>
-      <c r="Q66" s="6"/>
-      <c r="R66" s="6"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="4"/>
+      <c r="Q66" s="4"/>
+      <c r="R66" s="4"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
@@ -4671,12 +4683,12 @@
         <f t="shared" ref="K67:K130" si="7">IF(AND(F67=0, G67=0),1,0)</f>
         <v>1</v>
       </c>
-      <c r="M67" s="6"/>
-      <c r="N67" s="6"/>
-      <c r="O67" s="6"/>
-      <c r="P67" s="6"/>
-      <c r="Q67" s="6"/>
-      <c r="R67" s="6"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="4"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
@@ -4716,12 +4728,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M68" s="6"/>
-      <c r="N68" s="6"/>
-      <c r="O68" s="6"/>
-      <c r="P68" s="6"/>
-      <c r="Q68" s="6"/>
-      <c r="R68" s="6"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="4"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
@@ -4761,12 +4773,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
-      <c r="O69" s="6"/>
-      <c r="P69" s="6"/>
-      <c r="Q69" s="6"/>
-      <c r="R69" s="6"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
@@ -4806,12 +4818,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M70" s="8"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="6"/>
-      <c r="P70" s="6"/>
-      <c r="Q70" s="6"/>
-      <c r="R70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="4"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
@@ -4851,12 +4863,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
-      <c r="P71" s="6"/>
-      <c r="Q71" s="6"/>
-      <c r="R71" s="6"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="4"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
@@ -4896,12 +4908,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M72" s="6"/>
-      <c r="N72" s="6"/>
-      <c r="O72" s="6"/>
-      <c r="P72" s="6"/>
-      <c r="Q72" s="6"/>
-      <c r="R72" s="6"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="4"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
@@ -4941,12 +4953,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="6"/>
-      <c r="P73" s="6"/>
-      <c r="Q73" s="6"/>
-      <c r="R73" s="6"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="4"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
@@ -4986,12 +4998,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M74" s="6"/>
-      <c r="N74" s="6"/>
-      <c r="O74" s="6"/>
-      <c r="P74" s="6"/>
-      <c r="Q74" s="6"/>
-      <c r="R74" s="6"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="4"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
@@ -5031,12 +5043,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="6"/>
-      <c r="P75" s="6"/>
-      <c r="Q75" s="6"/>
-      <c r="R75" s="6"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
@@ -5076,12 +5088,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
-      <c r="O76" s="6"/>
-      <c r="P76" s="6"/>
-      <c r="Q76" s="6"/>
-      <c r="R76" s="6"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
+      <c r="Q76" s="4"/>
+      <c r="R76" s="4"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
@@ -5121,12 +5133,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M77" s="6"/>
-      <c r="N77" s="6"/>
-      <c r="O77" s="6"/>
-      <c r="P77" s="6"/>
-      <c r="Q77" s="6"/>
-      <c r="R77" s="6"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
@@ -5166,12 +5178,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6"/>
-      <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="4"/>
+      <c r="R78" s="4"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
@@ -5211,12 +5223,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M79" s="8"/>
-      <c r="N79" s="6"/>
-      <c r="O79" s="6"/>
-      <c r="P79" s="6"/>
-      <c r="Q79" s="6"/>
-      <c r="R79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="4"/>
+      <c r="R79" s="4"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
@@ -5256,12 +5268,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="6"/>
-      <c r="P80" s="6"/>
-      <c r="Q80" s="6"/>
-      <c r="R80" s="6"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
@@ -5301,12 +5313,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M81" s="6"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="6"/>
-      <c r="P81" s="6"/>
-      <c r="Q81" s="6"/>
-      <c r="R81" s="6"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
@@ -5346,12 +5358,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M82" s="6"/>
-      <c r="N82" s="6"/>
-      <c r="O82" s="6"/>
-      <c r="P82" s="6"/>
-      <c r="Q82" s="6"/>
-      <c r="R82" s="6"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="4"/>
+      <c r="R82" s="4"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
@@ -5391,12 +5403,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M83" s="6"/>
-      <c r="N83" s="6"/>
-      <c r="O83" s="6"/>
-      <c r="P83" s="6"/>
-      <c r="Q83" s="6"/>
-      <c r="R83" s="6"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="4"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
@@ -5436,12 +5448,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M84" s="6"/>
-      <c r="N84" s="6"/>
-      <c r="O84" s="6"/>
-      <c r="P84" s="6"/>
-      <c r="Q84" s="6"/>
-      <c r="R84" s="6"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="4"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
@@ -5481,12 +5493,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M85" s="6"/>
-      <c r="N85" s="6"/>
-      <c r="O85" s="6"/>
-      <c r="P85" s="6"/>
-      <c r="Q85" s="6"/>
-      <c r="R85" s="6"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="4"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
@@ -5526,12 +5538,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M86" s="6"/>
-      <c r="N86" s="6"/>
-      <c r="O86" s="6"/>
-      <c r="P86" s="6"/>
-      <c r="Q86" s="6"/>
-      <c r="R86" s="6"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="4"/>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
@@ -5571,12 +5583,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M87" s="6"/>
-      <c r="N87" s="6"/>
-      <c r="O87" s="6"/>
-      <c r="P87" s="6"/>
-      <c r="Q87" s="6"/>
-      <c r="R87" s="6"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="4"/>
+      <c r="R87" s="4"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
@@ -5616,12 +5628,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M88" s="6"/>
-      <c r="N88" s="6"/>
-      <c r="O88" s="6"/>
-      <c r="P88" s="6"/>
-      <c r="Q88" s="6"/>
-      <c r="R88" s="6"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
@@ -5661,12 +5673,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M89" s="6"/>
-      <c r="N89" s="6"/>
-      <c r="O89" s="6"/>
-      <c r="P89" s="6"/>
-      <c r="Q89" s="6"/>
-      <c r="R89" s="6"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
@@ -5706,12 +5718,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M90" s="6"/>
-      <c r="N90" s="6"/>
-      <c r="O90" s="6"/>
-      <c r="P90" s="6"/>
-      <c r="Q90" s="6"/>
-      <c r="R90" s="6"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="4"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="4"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
@@ -5751,12 +5763,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M91" s="6"/>
-      <c r="N91" s="6"/>
-      <c r="O91" s="6"/>
-      <c r="P91" s="6"/>
-      <c r="Q91" s="6"/>
-      <c r="R91" s="6"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="P91" s="4"/>
+      <c r="Q91" s="4"/>
+      <c r="R91" s="4"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
@@ -5796,12 +5808,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M92" s="6"/>
-      <c r="N92" s="6"/>
-      <c r="O92" s="6"/>
-      <c r="P92" s="6"/>
-      <c r="Q92" s="6"/>
-      <c r="R92" s="6"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="4"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="4"/>
+      <c r="Q92" s="4"/>
+      <c r="R92" s="4"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
@@ -5841,12 +5853,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M93" s="6"/>
-      <c r="N93" s="6"/>
-      <c r="O93" s="6"/>
-      <c r="P93" s="6"/>
-      <c r="Q93" s="6"/>
-      <c r="R93" s="6"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="4"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
@@ -5886,12 +5898,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M94" s="6"/>
-      <c r="N94" s="6"/>
-      <c r="O94" s="6"/>
-      <c r="P94" s="6"/>
-      <c r="Q94" s="6"/>
-      <c r="R94" s="6"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="4"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
@@ -5931,12 +5943,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M95" s="6"/>
-      <c r="N95" s="6"/>
-      <c r="O95" s="6"/>
-      <c r="P95" s="6"/>
-      <c r="Q95" s="6"/>
-      <c r="R95" s="6"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="4"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
@@ -5976,12 +5988,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M96" s="6"/>
-      <c r="N96" s="6"/>
-      <c r="O96" s="6"/>
-      <c r="P96" s="6"/>
-      <c r="Q96" s="6"/>
-      <c r="R96" s="6"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="4"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
@@ -6021,12 +6033,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M97" s="6"/>
-      <c r="N97" s="6"/>
-      <c r="O97" s="6"/>
-      <c r="P97" s="6"/>
-      <c r="Q97" s="6"/>
-      <c r="R97" s="6"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="4"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
@@ -6066,12 +6078,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M98" s="6"/>
-      <c r="N98" s="6"/>
-      <c r="O98" s="6"/>
-      <c r="P98" s="6"/>
-      <c r="Q98" s="6"/>
-      <c r="R98" s="6"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4"/>
+      <c r="Q98" s="4"/>
+      <c r="R98" s="4"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
@@ -6111,12 +6123,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M99" s="6"/>
-      <c r="N99" s="6"/>
-      <c r="O99" s="6"/>
-      <c r="P99" s="6"/>
-      <c r="Q99" s="6"/>
-      <c r="R99" s="6"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+      <c r="P99" s="4"/>
+      <c r="Q99" s="4"/>
+      <c r="R99" s="4"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
@@ -6156,12 +6168,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M100" s="6"/>
-      <c r="N100" s="6"/>
-      <c r="O100" s="6"/>
-      <c r="P100" s="6"/>
-      <c r="Q100" s="6"/>
-      <c r="R100" s="6"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="4"/>
+      <c r="Q100" s="4"/>
+      <c r="R100" s="4"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
@@ -6201,12 +6213,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M101" s="6"/>
-      <c r="N101" s="6"/>
-      <c r="O101" s="6"/>
-      <c r="P101" s="6"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="6"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
+      <c r="P101" s="4"/>
+      <c r="Q101" s="4"/>
+      <c r="R101" s="4"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
@@ -6246,12 +6258,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M102" s="6"/>
-      <c r="N102" s="6"/>
-      <c r="O102" s="6"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="6"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="4"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
@@ -6291,12 +6303,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M103" s="6"/>
-      <c r="N103" s="6"/>
-      <c r="O103" s="6"/>
-      <c r="P103" s="6"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="6"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="4"/>
+      <c r="O103" s="4"/>
+      <c r="P103" s="4"/>
+      <c r="Q103" s="4"/>
+      <c r="R103" s="4"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
@@ -6336,12 +6348,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M104" s="6"/>
-      <c r="N104" s="6"/>
-      <c r="O104" s="6"/>
-      <c r="P104" s="6"/>
-      <c r="Q104" s="6"/>
-      <c r="R104" s="6"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="4"/>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
@@ -6381,12 +6393,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M105" s="6"/>
-      <c r="N105" s="6"/>
-      <c r="O105" s="6"/>
-      <c r="P105" s="6"/>
-      <c r="Q105" s="6"/>
-      <c r="R105" s="6"/>
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="4"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
@@ -6426,12 +6438,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M106" s="6"/>
-      <c r="N106" s="6"/>
-      <c r="O106" s="6"/>
-      <c r="P106" s="6"/>
-      <c r="Q106" s="6"/>
-      <c r="R106" s="6"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="4"/>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
@@ -6471,12 +6483,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M107" s="6"/>
-      <c r="N107" s="6"/>
-      <c r="O107" s="6"/>
-      <c r="P107" s="6"/>
-      <c r="Q107" s="6"/>
-      <c r="R107" s="6"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="4"/>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
@@ -6516,12 +6528,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M108" s="6"/>
-      <c r="N108" s="6"/>
-      <c r="O108" s="6"/>
-      <c r="P108" s="6"/>
-      <c r="Q108" s="6"/>
-      <c r="R108" s="6"/>
+      <c r="M108" s="4"/>
+      <c r="N108" s="4"/>
+      <c r="O108" s="4"/>
+      <c r="P108" s="4"/>
+      <c r="Q108" s="4"/>
+      <c r="R108" s="4"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
@@ -6561,12 +6573,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M109" s="6"/>
-      <c r="N109" s="6"/>
-      <c r="O109" s="6"/>
-      <c r="P109" s="6"/>
-      <c r="Q109" s="6"/>
-      <c r="R109" s="6"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="4"/>
+      <c r="O109" s="4"/>
+      <c r="P109" s="4"/>
+      <c r="Q109" s="4"/>
+      <c r="R109" s="4"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
@@ -6606,12 +6618,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M110" s="6"/>
-      <c r="N110" s="6"/>
-      <c r="O110" s="6"/>
-      <c r="P110" s="6"/>
-      <c r="Q110" s="6"/>
-      <c r="R110" s="6"/>
+      <c r="M110" s="4"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="4"/>
+      <c r="P110" s="4"/>
+      <c r="Q110" s="4"/>
+      <c r="R110" s="4"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
@@ -6651,12 +6663,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M111" s="6"/>
-      <c r="N111" s="6"/>
-      <c r="O111" s="6"/>
-      <c r="P111" s="6"/>
-      <c r="Q111" s="6"/>
-      <c r="R111" s="6"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="4"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
@@ -6696,12 +6708,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M112" s="6"/>
-      <c r="N112" s="6"/>
-      <c r="O112" s="6"/>
-      <c r="P112" s="6"/>
-      <c r="Q112" s="6"/>
-      <c r="R112" s="6"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="4"/>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
@@ -6741,12 +6753,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M113" s="6"/>
-      <c r="N113" s="6"/>
-      <c r="O113" s="6"/>
-      <c r="P113" s="6"/>
-      <c r="Q113" s="6"/>
-      <c r="R113" s="6"/>
+      <c r="M113" s="4"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="4"/>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
@@ -6786,12 +6798,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M114" s="6"/>
-      <c r="N114" s="6"/>
-      <c r="O114" s="6"/>
-      <c r="P114" s="6"/>
-      <c r="Q114" s="6"/>
-      <c r="R114" s="6"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4"/>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
@@ -6831,12 +6843,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M115" s="6"/>
-      <c r="N115" s="6"/>
-      <c r="O115" s="6"/>
-      <c r="P115" s="6"/>
-      <c r="Q115" s="6"/>
-      <c r="R115" s="6"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="4"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
@@ -6876,12 +6888,12 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M116" s="6"/>
-      <c r="N116" s="6"/>
-      <c r="O116" s="6"/>
-      <c r="P116" s="6"/>
-      <c r="Q116" s="6"/>
-      <c r="R116" s="6"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="4"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="4"/>
+      <c r="Q116" s="4"/>
+      <c r="R116" s="4"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
@@ -6921,12 +6933,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M117" s="6"/>
-      <c r="N117" s="6"/>
-      <c r="O117" s="6"/>
-      <c r="P117" s="6"/>
-      <c r="Q117" s="6"/>
-      <c r="R117" s="6"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="4"/>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
@@ -6966,12 +6978,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M118" s="6"/>
-      <c r="N118" s="6"/>
-      <c r="O118" s="6"/>
-      <c r="P118" s="6"/>
-      <c r="Q118" s="6"/>
-      <c r="R118" s="6"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
@@ -7011,12 +7023,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M119" s="6"/>
-      <c r="N119" s="6"/>
-      <c r="O119" s="6"/>
-      <c r="P119" s="6"/>
-      <c r="Q119" s="6"/>
-      <c r="R119" s="6"/>
+      <c r="M119" s="4"/>
+      <c r="N119" s="4"/>
+      <c r="O119" s="4"/>
+      <c r="P119" s="4"/>
+      <c r="Q119" s="4"/>
+      <c r="R119" s="4"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
@@ -7056,12 +7068,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M120" s="6"/>
-      <c r="N120" s="6"/>
-      <c r="O120" s="6"/>
-      <c r="P120" s="6"/>
-      <c r="Q120" s="6"/>
-      <c r="R120" s="6"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="4"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="4"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
@@ -7101,12 +7113,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M121" s="6"/>
-      <c r="N121" s="6"/>
-      <c r="O121" s="6"/>
-      <c r="P121" s="6"/>
-      <c r="Q121" s="6"/>
-      <c r="R121" s="6"/>
+      <c r="M121" s="4"/>
+      <c r="N121" s="4"/>
+      <c r="O121" s="4"/>
+      <c r="P121" s="4"/>
+      <c r="Q121" s="4"/>
+      <c r="R121" s="4"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
@@ -7146,12 +7158,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M122" s="6"/>
-      <c r="N122" s="6"/>
-      <c r="O122" s="6"/>
-      <c r="P122" s="6"/>
-      <c r="Q122" s="6"/>
-      <c r="R122" s="6"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="4"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="4"/>
+      <c r="R122" s="4"/>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
@@ -7191,12 +7203,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M123" s="6"/>
-      <c r="N123" s="6"/>
-      <c r="O123" s="6"/>
-      <c r="P123" s="6"/>
-      <c r="Q123" s="6"/>
-      <c r="R123" s="6"/>
+      <c r="M123" s="4"/>
+      <c r="N123" s="4"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
+      <c r="Q123" s="4"/>
+      <c r="R123" s="4"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
@@ -7236,12 +7248,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M124" s="6"/>
-      <c r="N124" s="6"/>
-      <c r="O124" s="6"/>
-      <c r="P124" s="6"/>
-      <c r="Q124" s="6"/>
-      <c r="R124" s="6"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="4"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4"/>
+      <c r="Q124" s="4"/>
+      <c r="R124" s="4"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
@@ -7281,12 +7293,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M125" s="6"/>
-      <c r="N125" s="6"/>
-      <c r="O125" s="6"/>
-      <c r="P125" s="6"/>
-      <c r="Q125" s="6"/>
-      <c r="R125" s="6"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4"/>
+      <c r="P125" s="4"/>
+      <c r="Q125" s="4"/>
+      <c r="R125" s="4"/>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
@@ -7326,12 +7338,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M126" s="6"/>
-      <c r="N126" s="6"/>
-      <c r="O126" s="6"/>
-      <c r="P126" s="6"/>
-      <c r="Q126" s="6"/>
-      <c r="R126" s="6"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="4"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="4"/>
+      <c r="Q126" s="4"/>
+      <c r="R126" s="4"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
@@ -7371,12 +7383,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M127" s="6"/>
-      <c r="N127" s="6"/>
-      <c r="O127" s="6"/>
-      <c r="P127" s="6"/>
-      <c r="Q127" s="6"/>
-      <c r="R127" s="6"/>
+      <c r="M127" s="4"/>
+      <c r="N127" s="4"/>
+      <c r="O127" s="4"/>
+      <c r="P127" s="4"/>
+      <c r="Q127" s="4"/>
+      <c r="R127" s="4"/>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
@@ -7416,12 +7428,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M128" s="6"/>
-      <c r="N128" s="6"/>
-      <c r="O128" s="6"/>
-      <c r="P128" s="6"/>
-      <c r="Q128" s="6"/>
-      <c r="R128" s="6"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="4"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="4"/>
+      <c r="R128" s="4"/>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
@@ -7461,12 +7473,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M129" s="6"/>
-      <c r="N129" s="6"/>
-      <c r="O129" s="6"/>
-      <c r="P129" s="6"/>
-      <c r="Q129" s="6"/>
-      <c r="R129" s="6"/>
+      <c r="M129" s="4"/>
+      <c r="N129" s="4"/>
+      <c r="O129" s="4"/>
+      <c r="P129" s="4"/>
+      <c r="Q129" s="4"/>
+      <c r="R129" s="4"/>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
@@ -7506,12 +7518,12 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="M130" s="6"/>
-      <c r="N130" s="6"/>
-      <c r="O130" s="6"/>
-      <c r="P130" s="6"/>
-      <c r="Q130" s="6"/>
-      <c r="R130" s="6"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="4"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="4"/>
+      <c r="Q130" s="4"/>
+      <c r="R130" s="4"/>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
@@ -7551,12 +7563,12 @@
         <f t="shared" ref="K131:K185" si="11">IF(AND(F131=0, G131=0),1,0)</f>
         <v>0</v>
       </c>
-      <c r="M131" s="6"/>
-      <c r="N131" s="6"/>
-      <c r="O131" s="6"/>
-      <c r="P131" s="6"/>
-      <c r="Q131" s="6"/>
-      <c r="R131" s="6"/>
+      <c r="M131" s="4"/>
+      <c r="N131" s="4"/>
+      <c r="O131" s="4"/>
+      <c r="P131" s="4"/>
+      <c r="Q131" s="4"/>
+      <c r="R131" s="4"/>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
@@ -7596,12 +7608,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M132" s="6"/>
-      <c r="N132" s="6"/>
-      <c r="O132" s="6"/>
-      <c r="P132" s="6"/>
-      <c r="Q132" s="6"/>
-      <c r="R132" s="6"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="4"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="4"/>
+      <c r="Q132" s="4"/>
+      <c r="R132" s="4"/>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
@@ -7641,12 +7653,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M133" s="6"/>
-      <c r="N133" s="6"/>
-      <c r="O133" s="6"/>
-      <c r="P133" s="6"/>
-      <c r="Q133" s="6"/>
-      <c r="R133" s="6"/>
+      <c r="M133" s="4"/>
+      <c r="N133" s="4"/>
+      <c r="O133" s="4"/>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="4"/>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
@@ -7686,12 +7698,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M134" s="6"/>
-      <c r="N134" s="6"/>
-      <c r="O134" s="6"/>
-      <c r="P134" s="6"/>
-      <c r="Q134" s="6"/>
-      <c r="R134" s="6"/>
+      <c r="M134" s="4"/>
+      <c r="N134" s="4"/>
+      <c r="O134" s="4"/>
+      <c r="P134" s="4"/>
+      <c r="Q134" s="4"/>
+      <c r="R134" s="4"/>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
@@ -7731,12 +7743,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M135" s="6"/>
-      <c r="N135" s="6"/>
-      <c r="O135" s="6"/>
-      <c r="P135" s="6"/>
-      <c r="Q135" s="6"/>
-      <c r="R135" s="6"/>
+      <c r="M135" s="4"/>
+      <c r="N135" s="4"/>
+      <c r="O135" s="4"/>
+      <c r="P135" s="4"/>
+      <c r="Q135" s="4"/>
+      <c r="R135" s="4"/>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
@@ -7776,12 +7788,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M136" s="6"/>
-      <c r="N136" s="6"/>
-      <c r="O136" s="6"/>
-      <c r="P136" s="6"/>
-      <c r="Q136" s="6"/>
-      <c r="R136" s="6"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="4"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="4"/>
+      <c r="Q136" s="4"/>
+      <c r="R136" s="4"/>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
@@ -7821,12 +7833,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M137" s="6"/>
-      <c r="N137" s="6"/>
-      <c r="O137" s="6"/>
-      <c r="P137" s="6"/>
-      <c r="Q137" s="6"/>
-      <c r="R137" s="6"/>
+      <c r="M137" s="4"/>
+      <c r="N137" s="4"/>
+      <c r="O137" s="4"/>
+      <c r="P137" s="4"/>
+      <c r="Q137" s="4"/>
+      <c r="R137" s="4"/>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
@@ -7866,12 +7878,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M138" s="6"/>
-      <c r="N138" s="6"/>
-      <c r="O138" s="6"/>
-      <c r="P138" s="6"/>
-      <c r="Q138" s="6"/>
-      <c r="R138" s="6"/>
+      <c r="M138" s="4"/>
+      <c r="N138" s="4"/>
+      <c r="O138" s="4"/>
+      <c r="P138" s="4"/>
+      <c r="Q138" s="4"/>
+      <c r="R138" s="4"/>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
@@ -7911,12 +7923,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M139" s="6"/>
-      <c r="N139" s="6"/>
-      <c r="O139" s="6"/>
-      <c r="P139" s="6"/>
-      <c r="Q139" s="6"/>
-      <c r="R139" s="6"/>
+      <c r="M139" s="4"/>
+      <c r="N139" s="4"/>
+      <c r="O139" s="4"/>
+      <c r="P139" s="4"/>
+      <c r="Q139" s="4"/>
+      <c r="R139" s="4"/>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
@@ -7956,12 +7968,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M140" s="6"/>
-      <c r="N140" s="6"/>
-      <c r="O140" s="6"/>
-      <c r="P140" s="6"/>
-      <c r="Q140" s="6"/>
-      <c r="R140" s="6"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="4"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="4"/>
+      <c r="Q140" s="4"/>
+      <c r="R140" s="4"/>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
@@ -8001,12 +8013,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M141" s="6"/>
-      <c r="N141" s="6"/>
-      <c r="O141" s="6"/>
-      <c r="P141" s="6"/>
-      <c r="Q141" s="6"/>
-      <c r="R141" s="6"/>
+      <c r="M141" s="4"/>
+      <c r="N141" s="4"/>
+      <c r="O141" s="4"/>
+      <c r="P141" s="4"/>
+      <c r="Q141" s="4"/>
+      <c r="R141" s="4"/>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
@@ -8046,12 +8058,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M142" s="6"/>
-      <c r="N142" s="6"/>
-      <c r="O142" s="6"/>
-      <c r="P142" s="6"/>
-      <c r="Q142" s="6"/>
-      <c r="R142" s="6"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="4"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="4"/>
+      <c r="Q142" s="4"/>
+      <c r="R142" s="4"/>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
@@ -8091,12 +8103,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M143" s="6"/>
-      <c r="N143" s="6"/>
-      <c r="O143" s="6"/>
-      <c r="P143" s="6"/>
-      <c r="Q143" s="6"/>
-      <c r="R143" s="6"/>
+      <c r="M143" s="4"/>
+      <c r="N143" s="4"/>
+      <c r="O143" s="4"/>
+      <c r="P143" s="4"/>
+      <c r="Q143" s="4"/>
+      <c r="R143" s="4"/>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
@@ -8136,12 +8148,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M144" s="6"/>
-      <c r="N144" s="6"/>
-      <c r="O144" s="6"/>
-      <c r="P144" s="6"/>
-      <c r="Q144" s="6"/>
-      <c r="R144" s="6"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="4"/>
+      <c r="Q144" s="4"/>
+      <c r="R144" s="4"/>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
@@ -8181,12 +8193,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M145" s="6"/>
-      <c r="N145" s="6"/>
-      <c r="O145" s="6"/>
-      <c r="P145" s="6"/>
-      <c r="Q145" s="6"/>
-      <c r="R145" s="6"/>
+      <c r="M145" s="4"/>
+      <c r="N145" s="4"/>
+      <c r="O145" s="4"/>
+      <c r="P145" s="4"/>
+      <c r="Q145" s="4"/>
+      <c r="R145" s="4"/>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
@@ -8226,12 +8238,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M146" s="6"/>
-      <c r="N146" s="6"/>
-      <c r="O146" s="6"/>
-      <c r="P146" s="6"/>
-      <c r="Q146" s="6"/>
-      <c r="R146" s="6"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="4"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4"/>
+      <c r="R146" s="4"/>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
@@ -8271,12 +8283,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M147" s="6"/>
-      <c r="N147" s="6"/>
-      <c r="O147" s="6"/>
-      <c r="P147" s="6"/>
-      <c r="Q147" s="6"/>
-      <c r="R147" s="6"/>
+      <c r="M147" s="4"/>
+      <c r="N147" s="4"/>
+      <c r="O147" s="4"/>
+      <c r="P147" s="4"/>
+      <c r="Q147" s="4"/>
+      <c r="R147" s="4"/>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
@@ -8316,12 +8328,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M148" s="6"/>
-      <c r="N148" s="6"/>
-      <c r="O148" s="6"/>
-      <c r="P148" s="6"/>
-      <c r="Q148" s="6"/>
-      <c r="R148" s="6"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="4"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="4"/>
+      <c r="Q148" s="4"/>
+      <c r="R148" s="4"/>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
@@ -8361,12 +8373,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M149" s="6"/>
-      <c r="N149" s="6"/>
-      <c r="O149" s="6"/>
-      <c r="P149" s="6"/>
-      <c r="Q149" s="6"/>
-      <c r="R149" s="6"/>
+      <c r="M149" s="4"/>
+      <c r="N149" s="4"/>
+      <c r="O149" s="4"/>
+      <c r="P149" s="4"/>
+      <c r="Q149" s="4"/>
+      <c r="R149" s="4"/>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
@@ -8406,12 +8418,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M150" s="6"/>
-      <c r="N150" s="6"/>
-      <c r="O150" s="6"/>
-      <c r="P150" s="6"/>
-      <c r="Q150" s="6"/>
-      <c r="R150" s="6"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="4"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="4"/>
+      <c r="Q150" s="4"/>
+      <c r="R150" s="4"/>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
@@ -8451,12 +8463,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M151" s="6"/>
-      <c r="N151" s="6"/>
-      <c r="O151" s="6"/>
-      <c r="P151" s="6"/>
-      <c r="Q151" s="6"/>
-      <c r="R151" s="6"/>
+      <c r="M151" s="4"/>
+      <c r="N151" s="4"/>
+      <c r="O151" s="4"/>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4"/>
+      <c r="R151" s="4"/>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
@@ -8496,12 +8508,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M152" s="6"/>
-      <c r="N152" s="6"/>
-      <c r="O152" s="6"/>
-      <c r="P152" s="6"/>
-      <c r="Q152" s="6"/>
-      <c r="R152" s="6"/>
+      <c r="M152" s="4"/>
+      <c r="N152" s="4"/>
+      <c r="O152" s="4"/>
+      <c r="P152" s="4"/>
+      <c r="Q152" s="4"/>
+      <c r="R152" s="4"/>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
@@ -8541,12 +8553,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M153" s="6"/>
-      <c r="N153" s="6"/>
-      <c r="O153" s="6"/>
-      <c r="P153" s="6"/>
-      <c r="Q153" s="6"/>
-      <c r="R153" s="6"/>
+      <c r="M153" s="4"/>
+      <c r="N153" s="4"/>
+      <c r="O153" s="4"/>
+      <c r="P153" s="4"/>
+      <c r="Q153" s="4"/>
+      <c r="R153" s="4"/>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
@@ -8586,12 +8598,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M154" s="6"/>
-      <c r="N154" s="6"/>
-      <c r="O154" s="6"/>
-      <c r="P154" s="6"/>
-      <c r="Q154" s="6"/>
-      <c r="R154" s="6"/>
+      <c r="M154" s="4"/>
+      <c r="N154" s="4"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="4"/>
+      <c r="Q154" s="4"/>
+      <c r="R154" s="4"/>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
@@ -8631,12 +8643,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M155" s="6"/>
-      <c r="N155" s="6"/>
-      <c r="O155" s="6"/>
-      <c r="P155" s="6"/>
-      <c r="Q155" s="6"/>
-      <c r="R155" s="6"/>
+      <c r="M155" s="4"/>
+      <c r="N155" s="4"/>
+      <c r="O155" s="4"/>
+      <c r="P155" s="4"/>
+      <c r="Q155" s="4"/>
+      <c r="R155" s="4"/>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
@@ -8676,12 +8688,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M156" s="6"/>
-      <c r="N156" s="6"/>
-      <c r="O156" s="6"/>
-      <c r="P156" s="6"/>
-      <c r="Q156" s="6"/>
-      <c r="R156" s="6"/>
+      <c r="M156" s="4"/>
+      <c r="N156" s="4"/>
+      <c r="O156" s="4"/>
+      <c r="P156" s="4"/>
+      <c r="Q156" s="4"/>
+      <c r="R156" s="4"/>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
@@ -8721,12 +8733,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M157" s="6"/>
-      <c r="N157" s="6"/>
-      <c r="O157" s="6"/>
-      <c r="P157" s="6"/>
-      <c r="Q157" s="6"/>
-      <c r="R157" s="6"/>
+      <c r="M157" s="4"/>
+      <c r="N157" s="4"/>
+      <c r="O157" s="4"/>
+      <c r="P157" s="4"/>
+      <c r="Q157" s="4"/>
+      <c r="R157" s="4"/>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
@@ -8766,12 +8778,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M158" s="6"/>
-      <c r="N158" s="6"/>
-      <c r="O158" s="6"/>
-      <c r="P158" s="6"/>
-      <c r="Q158" s="6"/>
-      <c r="R158" s="6"/>
+      <c r="M158" s="4"/>
+      <c r="N158" s="4"/>
+      <c r="O158" s="4"/>
+      <c r="P158" s="4"/>
+      <c r="Q158" s="4"/>
+      <c r="R158" s="4"/>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
@@ -8811,12 +8823,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M159" s="6"/>
-      <c r="N159" s="6"/>
-      <c r="O159" s="6"/>
-      <c r="P159" s="6"/>
-      <c r="Q159" s="6"/>
-      <c r="R159" s="6"/>
+      <c r="M159" s="4"/>
+      <c r="N159" s="4"/>
+      <c r="O159" s="4"/>
+      <c r="P159" s="4"/>
+      <c r="Q159" s="4"/>
+      <c r="R159" s="4"/>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
@@ -8856,12 +8868,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M160" s="6"/>
-      <c r="N160" s="6"/>
-      <c r="O160" s="6"/>
-      <c r="P160" s="6"/>
-      <c r="Q160" s="6"/>
-      <c r="R160" s="6"/>
+      <c r="M160" s="4"/>
+      <c r="N160" s="4"/>
+      <c r="O160" s="4"/>
+      <c r="P160" s="4"/>
+      <c r="Q160" s="4"/>
+      <c r="R160" s="4"/>
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
@@ -8901,12 +8913,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M161" s="6"/>
-      <c r="N161" s="6"/>
-      <c r="O161" s="6"/>
-      <c r="P161" s="6"/>
-      <c r="Q161" s="6"/>
-      <c r="R161" s="6"/>
+      <c r="M161" s="4"/>
+      <c r="N161" s="4"/>
+      <c r="O161" s="4"/>
+      <c r="P161" s="4"/>
+      <c r="Q161" s="4"/>
+      <c r="R161" s="4"/>
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
@@ -8946,12 +8958,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M162" s="6"/>
-      <c r="N162" s="6"/>
-      <c r="O162" s="6"/>
-      <c r="P162" s="6"/>
-      <c r="Q162" s="6"/>
-      <c r="R162" s="6"/>
+      <c r="M162" s="4"/>
+      <c r="N162" s="4"/>
+      <c r="O162" s="4"/>
+      <c r="P162" s="4"/>
+      <c r="Q162" s="4"/>
+      <c r="R162" s="4"/>
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
@@ -8991,12 +9003,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M163" s="6"/>
-      <c r="N163" s="6"/>
-      <c r="O163" s="6"/>
-      <c r="P163" s="6"/>
-      <c r="Q163" s="6"/>
-      <c r="R163" s="6"/>
+      <c r="M163" s="4"/>
+      <c r="N163" s="4"/>
+      <c r="O163" s="4"/>
+      <c r="P163" s="4"/>
+      <c r="Q163" s="4"/>
+      <c r="R163" s="4"/>
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
@@ -9036,12 +9048,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M164" s="6"/>
-      <c r="N164" s="6"/>
-      <c r="O164" s="6"/>
-      <c r="P164" s="6"/>
-      <c r="Q164" s="6"/>
-      <c r="R164" s="6"/>
+      <c r="M164" s="4"/>
+      <c r="N164" s="4"/>
+      <c r="O164" s="4"/>
+      <c r="P164" s="4"/>
+      <c r="Q164" s="4"/>
+      <c r="R164" s="4"/>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
@@ -9081,12 +9093,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M165" s="6"/>
-      <c r="N165" s="6"/>
-      <c r="O165" s="6"/>
-      <c r="P165" s="6"/>
-      <c r="Q165" s="6"/>
-      <c r="R165" s="6"/>
+      <c r="M165" s="4"/>
+      <c r="N165" s="4"/>
+      <c r="O165" s="4"/>
+      <c r="P165" s="4"/>
+      <c r="Q165" s="4"/>
+      <c r="R165" s="4"/>
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
@@ -9126,12 +9138,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M166" s="6"/>
-      <c r="N166" s="6"/>
-      <c r="O166" s="6"/>
-      <c r="P166" s="6"/>
-      <c r="Q166" s="6"/>
-      <c r="R166" s="6"/>
+      <c r="M166" s="4"/>
+      <c r="N166" s="4"/>
+      <c r="O166" s="4"/>
+      <c r="P166" s="4"/>
+      <c r="Q166" s="4"/>
+      <c r="R166" s="4"/>
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
@@ -9171,12 +9183,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M167" s="6"/>
-      <c r="N167" s="6"/>
-      <c r="O167" s="6"/>
-      <c r="P167" s="6"/>
-      <c r="Q167" s="6"/>
-      <c r="R167" s="6"/>
+      <c r="M167" s="4"/>
+      <c r="N167" s="4"/>
+      <c r="O167" s="4"/>
+      <c r="P167" s="4"/>
+      <c r="Q167" s="4"/>
+      <c r="R167" s="4"/>
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
@@ -9216,12 +9228,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M168" s="6"/>
-      <c r="N168" s="6"/>
-      <c r="O168" s="6"/>
-      <c r="P168" s="6"/>
-      <c r="Q168" s="6"/>
-      <c r="R168" s="6"/>
+      <c r="M168" s="4"/>
+      <c r="N168" s="4"/>
+      <c r="O168" s="4"/>
+      <c r="P168" s="4"/>
+      <c r="Q168" s="4"/>
+      <c r="R168" s="4"/>
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
@@ -9261,12 +9273,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M169" s="6"/>
-      <c r="N169" s="6"/>
-      <c r="O169" s="6"/>
-      <c r="P169" s="6"/>
-      <c r="Q169" s="6"/>
-      <c r="R169" s="6"/>
+      <c r="M169" s="4"/>
+      <c r="N169" s="4"/>
+      <c r="O169" s="4"/>
+      <c r="P169" s="4"/>
+      <c r="Q169" s="4"/>
+      <c r="R169" s="4"/>
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
@@ -9306,12 +9318,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M170" s="6"/>
-      <c r="N170" s="6"/>
-      <c r="O170" s="6"/>
-      <c r="P170" s="6"/>
-      <c r="Q170" s="6"/>
-      <c r="R170" s="6"/>
+      <c r="M170" s="4"/>
+      <c r="N170" s="4"/>
+      <c r="O170" s="4"/>
+      <c r="P170" s="4"/>
+      <c r="Q170" s="4"/>
+      <c r="R170" s="4"/>
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
@@ -9351,12 +9363,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M171" s="6"/>
-      <c r="N171" s="6"/>
-      <c r="O171" s="6"/>
-      <c r="P171" s="6"/>
-      <c r="Q171" s="6"/>
-      <c r="R171" s="6"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
+      <c r="O171" s="4"/>
+      <c r="P171" s="4"/>
+      <c r="Q171" s="4"/>
+      <c r="R171" s="4"/>
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
@@ -9396,12 +9408,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M172" s="6"/>
-      <c r="N172" s="6"/>
-      <c r="O172" s="6"/>
-      <c r="P172" s="6"/>
-      <c r="Q172" s="6"/>
-      <c r="R172" s="6"/>
+      <c r="M172" s="4"/>
+      <c r="N172" s="4"/>
+      <c r="O172" s="4"/>
+      <c r="P172" s="4"/>
+      <c r="Q172" s="4"/>
+      <c r="R172" s="4"/>
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
@@ -9441,12 +9453,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M173" s="6"/>
-      <c r="N173" s="6"/>
-      <c r="O173" s="6"/>
-      <c r="P173" s="6"/>
-      <c r="Q173" s="6"/>
-      <c r="R173" s="6"/>
+      <c r="M173" s="4"/>
+      <c r="N173" s="4"/>
+      <c r="O173" s="4"/>
+      <c r="P173" s="4"/>
+      <c r="Q173" s="4"/>
+      <c r="R173" s="4"/>
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
@@ -9486,12 +9498,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M174" s="6"/>
-      <c r="N174" s="6"/>
-      <c r="O174" s="6"/>
-      <c r="P174" s="6"/>
-      <c r="Q174" s="6"/>
-      <c r="R174" s="6"/>
+      <c r="M174" s="4"/>
+      <c r="N174" s="4"/>
+      <c r="O174" s="4"/>
+      <c r="P174" s="4"/>
+      <c r="Q174" s="4"/>
+      <c r="R174" s="4"/>
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
@@ -9531,12 +9543,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M175" s="6"/>
-      <c r="N175" s="6"/>
-      <c r="O175" s="6"/>
-      <c r="P175" s="6"/>
-      <c r="Q175" s="6"/>
-      <c r="R175" s="6"/>
+      <c r="M175" s="4"/>
+      <c r="N175" s="4"/>
+      <c r="O175" s="4"/>
+      <c r="P175" s="4"/>
+      <c r="Q175" s="4"/>
+      <c r="R175" s="4"/>
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
@@ -9576,12 +9588,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M176" s="6"/>
-      <c r="N176" s="6"/>
-      <c r="O176" s="6"/>
-      <c r="P176" s="6"/>
-      <c r="Q176" s="6"/>
-      <c r="R176" s="6"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="4"/>
+      <c r="P176" s="4"/>
+      <c r="Q176" s="4"/>
+      <c r="R176" s="4"/>
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
@@ -9621,12 +9633,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M177" s="6"/>
-      <c r="N177" s="6"/>
-      <c r="O177" s="6"/>
-      <c r="P177" s="6"/>
-      <c r="Q177" s="6"/>
-      <c r="R177" s="6"/>
+      <c r="M177" s="4"/>
+      <c r="N177" s="4"/>
+      <c r="O177" s="4"/>
+      <c r="P177" s="4"/>
+      <c r="Q177" s="4"/>
+      <c r="R177" s="4"/>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
@@ -9666,12 +9678,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M178" s="6"/>
-      <c r="N178" s="6"/>
-      <c r="O178" s="6"/>
-      <c r="P178" s="6"/>
-      <c r="Q178" s="6"/>
-      <c r="R178" s="6"/>
+      <c r="M178" s="4"/>
+      <c r="N178" s="4"/>
+      <c r="O178" s="4"/>
+      <c r="P178" s="4"/>
+      <c r="Q178" s="4"/>
+      <c r="R178" s="4"/>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
@@ -9711,12 +9723,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M179" s="6"/>
-      <c r="N179" s="6"/>
-      <c r="O179" s="6"/>
-      <c r="P179" s="6"/>
-      <c r="Q179" s="6"/>
-      <c r="R179" s="6"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
+      <c r="P179" s="4"/>
+      <c r="Q179" s="4"/>
+      <c r="R179" s="4"/>
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
@@ -9756,12 +9768,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M180" s="6"/>
-      <c r="N180" s="6"/>
-      <c r="O180" s="6"/>
-      <c r="P180" s="6"/>
-      <c r="Q180" s="6"/>
-      <c r="R180" s="6"/>
+      <c r="M180" s="4"/>
+      <c r="N180" s="4"/>
+      <c r="O180" s="4"/>
+      <c r="P180" s="4"/>
+      <c r="Q180" s="4"/>
+      <c r="R180" s="4"/>
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
@@ -9801,12 +9813,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M181" s="6"/>
-      <c r="N181" s="6"/>
-      <c r="O181" s="6"/>
-      <c r="P181" s="6"/>
-      <c r="Q181" s="6"/>
-      <c r="R181" s="6"/>
+      <c r="M181" s="4"/>
+      <c r="N181" s="4"/>
+      <c r="O181" s="4"/>
+      <c r="P181" s="4"/>
+      <c r="Q181" s="4"/>
+      <c r="R181" s="4"/>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
@@ -9846,12 +9858,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M182" s="6"/>
-      <c r="N182" s="6"/>
-      <c r="O182" s="6"/>
-      <c r="P182" s="6"/>
-      <c r="Q182" s="6"/>
-      <c r="R182" s="6"/>
+      <c r="M182" s="4"/>
+      <c r="N182" s="4"/>
+      <c r="O182" s="4"/>
+      <c r="P182" s="4"/>
+      <c r="Q182" s="4"/>
+      <c r="R182" s="4"/>
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
@@ -9891,12 +9903,12 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M183" s="6"/>
-      <c r="N183" s="6"/>
-      <c r="O183" s="6"/>
-      <c r="P183" s="6"/>
-      <c r="Q183" s="6"/>
-      <c r="R183" s="6"/>
+      <c r="M183" s="4"/>
+      <c r="N183" s="4"/>
+      <c r="O183" s="4"/>
+      <c r="P183" s="4"/>
+      <c r="Q183" s="4"/>
+      <c r="R183" s="4"/>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
@@ -9936,12 +9948,12 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M184" s="6"/>
-      <c r="N184" s="6"/>
-      <c r="O184" s="6"/>
-      <c r="P184" s="6"/>
-      <c r="Q184" s="6"/>
-      <c r="R184" s="6"/>
+      <c r="M184" s="4"/>
+      <c r="N184" s="4"/>
+      <c r="O184" s="4"/>
+      <c r="P184" s="4"/>
+      <c r="Q184" s="4"/>
+      <c r="R184" s="4"/>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
@@ -9981,20 +9993,25 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="M185" s="6"/>
-      <c r="N185" s="6"/>
-      <c r="O185" s="6"/>
-      <c r="P185" s="6"/>
-      <c r="Q185" s="6"/>
-      <c r="R185" s="6"/>
+      <c r="M185" s="4"/>
+      <c r="N185" s="4"/>
+      <c r="O185" s="4"/>
+      <c r="P185" s="4"/>
+      <c r="Q185" s="4"/>
+      <c r="R185" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
     <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
+  <conditionalFormatting sqref="H1:I1048576">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -10008,8 +10025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59393675-1AD4-4B77-B567-61823439A5C9}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10039,7 +10056,7 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>383</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -10090,7 +10107,7 @@
         <f t="shared" ref="K2" si="3">IF(AND(F2=0, G2=0),1,0)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="9" t="s">
         <v>396</v>
       </c>
     </row>
@@ -10132,7 +10149,7 @@
         <f t="shared" ref="K3:K5" si="7">IF(AND(F3=0, G3=0),1,0)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="10" t="s">
         <v>397</v>
       </c>
     </row>
@@ -10174,7 +10191,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="10" t="s">
         <v>395</v>
       </c>
     </row>
@@ -10216,7 +10233,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="9" t="s">
         <v>396</v>
       </c>
     </row>
@@ -10258,7 +10275,7 @@
         <f t="shared" ref="K6:K7" si="11">IF(AND(F6=0, G6=0),1,0)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="8" t="s">
         <v>394</v>
       </c>
     </row>
@@ -10300,25 +10317,25 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="8" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="5" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="9" t="s">
         <v>397</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="8" t="s">
         <v>401</v>
       </c>
       <c r="L11">
@@ -10327,27 +10344,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:I3 H6:I1048576">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10357,10 +10374,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE01D7F2-835D-47EE-9059-24B873AC1FFE}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10447,7 +10464,7 @@
         <f t="shared" ref="K2" si="3">IF(AND(F2=0, G2=0),1,0)</f>
         <v>0</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="8" t="s">
         <v>391</v>
       </c>
     </row>
@@ -10489,7 +10506,7 @@
         <f t="shared" ref="K3:K4" si="7">IF(AND(F3=0, G3=0),1,0)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="8" t="s">
         <v>392</v>
       </c>
     </row>
@@ -10531,7 +10548,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="8" t="s">
         <v>391</v>
       </c>
     </row>
@@ -10573,7 +10590,7 @@
         <f t="shared" ref="K5:K6" si="11">IF(AND(F5=0, G5=0),1,0)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="8" t="s">
         <v>393</v>
       </c>
     </row>
@@ -10615,16 +10632,26 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="8" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="K8" s="7"/>
+      <c r="K8" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K9" s="8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K10" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>